<commit_message>
Slightly modified the board (but noch schematics) of the Arduino version. The new version is intended for a professionally etched board with plated through vias, silkscreen and all.
</commit_message>
<xml_diff>
--- a/SolarCharger_RevF_BOM.xlsx
+++ b/SolarCharger_RevF_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e83fb824b9dd0bd/EmbeddedSystems/eagle/SolarCharger/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfaes\OneDrive\EmbeddedSystems\eagle\SolarCharger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="8_{988B8D48-4016-4EDD-80EC-FD46F08DDBD3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{7B49178E-FE99-4098-9003-3080FE538F29}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="8_{988B8D48-4016-4EDD-80EC-FD46F08DDBD3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{7B49178E-FE99-4098-9003-3080FE538F29}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="28560" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$F$33</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$49</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -1385,7 +1385,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N31" sqref="N31"/>
+      <selection pane="bottomLeft" activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>